<commit_message>
Adding ecluded tags and and real time tags for suscribers
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/subscribers.xlsx
+++ b/epitweetr/inst/extdata/subscribers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">User</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">Topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excluded Topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real time Topics</t>
   </si>
   <si>
     <t xml:space="preserve">Regions</t>
@@ -142,10 +148,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:F2"/>
+  <dimension ref="B2:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:F5"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -172,6 +178,12 @@
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
1. Making data directory read only 2. Add disclaimer on country / territories 3. Allow user to customize coutries
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/subscribers.xlsx
+++ b/epitweetr/inst/extdata/subscribers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">User</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Regions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real time Regions</t>
   </si>
   <si>
     <t xml:space="preserve">Alert Slots</t>
@@ -148,10 +151,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:H2"/>
+  <dimension ref="B2:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -159,7 +162,9 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -183,6 +188,9 @@
       </c>
       <c r="H2" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Imprementing alerts related improvements 2. Fixing error preventing user only authentification to discard v2 api
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/subscribers.xlsx
+++ b/epitweetr/inst/extdata/subscribers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">User</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t xml:space="preserve">Alert Slots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One tweet alerts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topics ignoring 1 tweet alerts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regions ignoring 1 tweet alerts </t>
   </si>
 </sst>
 </file>
@@ -157,8 +166,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -247,20 +256,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:J9"/>
+  <dimension ref="B2:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:J3"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.67"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -287,6 +298,15 @@
       </c>
       <c r="J2" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,6 +319,9 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2"/>
@@ -310,6 +333,9 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2"/>
@@ -321,6 +347,9 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2"/>
@@ -332,6 +361,9 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2"/>
@@ -343,6 +375,9 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2"/>
@@ -354,6 +389,9 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2"/>
@@ -365,6 +403,9 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>